<commit_message>
adding new data TROY-DIANE, TROY-DIANE+BJ
git-svn-id: file://localhost/tmp/svn2git/svn@5369 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/troy/pstar/new_results.xlsx
+++ b/papers/troy/pstar/new_results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3200" yWindow="0" windowWidth="25600" windowHeight="16320" tabRatio="500"/>
+    <workbookView xWindow="1260" yWindow="0" windowWidth="25600" windowHeight="16360" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="19">
   <si>
     <t>wu-runtime avg</t>
   </si>
@@ -48,22 +48,34 @@
     <t>Startup time  (troy+bigjob+condor+filetranfer) with DIANE installations</t>
   </si>
   <si>
-    <t xml:space="preserve">1 test </t>
-  </si>
-  <si>
-    <t>wus</t>
-  </si>
-  <si>
     <t>Startup time  (troy+condor) with DIANE installations</t>
   </si>
   <si>
     <t>Startup time (troy+diane+bigjob+remote q time) with DIANE installations</t>
   </si>
   <si>
-    <t>2 test</t>
-  </si>
-  <si>
-    <t>3 test</t>
+    <t>1 node BJ + 1 node Diane</t>
+  </si>
+  <si>
+    <t>wu_1 runtime</t>
+  </si>
+  <si>
+    <t>wu_2 runtime</t>
+  </si>
+  <si>
+    <t>wu_3 runtime</t>
+  </si>
+  <si>
+    <t>wu_4 runtime</t>
+  </si>
+  <si>
+    <t>AVG</t>
+  </si>
+  <si>
+    <t>troy+diane start time+qtime</t>
+  </si>
+  <si>
+    <t>troy+BJ start time+qtime</t>
   </si>
 </sst>
 </file>
@@ -136,7 +148,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="62">
+  <cellStyleXfs count="114">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -199,8 +211,60 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyAlignment="1">
@@ -210,8 +274,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="62">
+  <cellStyles count="114">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -242,6 +312,32 @@
     <cellStyle name="Followed Hyperlink" xfId="57" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="63" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="65" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="67" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="69" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="71" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="73" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="75" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="77" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="79" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="81" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="83" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="85" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="87" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="89" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="91" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="93" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="95" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="97" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="99" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="101" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="103" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="105" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="107" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="109" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="111" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="113" builtinId="9" hidden="1"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
@@ -273,6 +369,32 @@
     <cellStyle name="Hyperlink" xfId="56" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="58" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="60" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="62" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="64" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="66" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="68" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="70" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="72" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="74" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="76" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="78" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="80" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="82" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="84" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="86" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="88" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="90" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="92" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="94" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="96" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="98" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="100" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="102" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="104" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="106" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="108" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="110" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="112" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -602,10 +724,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K40"/>
+  <dimension ref="A1:N42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="G44" sqref="G44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -616,13 +738,8 @@
     <col min="4" max="4" width="24.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="17" customHeight="1"/>
-    <row r="6" spans="1:11">
-      <c r="I6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="39" thickBot="1">
+    <row r="1" spans="1:13" ht="17" customHeight="1"/>
+    <row r="8" spans="1:13" ht="39" thickBot="1">
       <c r="A8" s="2" t="s">
         <v>1</v>
       </c>
@@ -638,17 +755,20 @@
       <c r="E8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I8" t="s">
-        <v>9</v>
-      </c>
-      <c r="J8" t="s">
+      <c r="J8" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="K8" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="K8" t="s">
+      <c r="L8" s="6" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" ht="16" thickTop="1">
+      <c r="M8" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="16" thickTop="1">
       <c r="C9">
         <v>81.040000000000006</v>
       </c>
@@ -658,17 +778,20 @@
       <c r="E9">
         <v>173.8</v>
       </c>
-      <c r="I9">
+      <c r="J9" s="1">
         <v>81.900000000000006</v>
       </c>
-      <c r="J9">
-        <v>87.52</v>
-      </c>
-      <c r="K9">
-        <v>82.13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11">
+      <c r="K9" s="1">
+        <v>81.900000000000006</v>
+      </c>
+      <c r="L9" s="1">
+        <v>81.900000000000006</v>
+      </c>
+      <c r="M9" s="1">
+        <v>81.900000000000006</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
       <c r="C10">
         <v>75.709999999999994</v>
       </c>
@@ -678,17 +801,20 @@
       <c r="E10">
         <v>168.59</v>
       </c>
-      <c r="I10">
-        <v>81.900000000000006</v>
-      </c>
-      <c r="J10">
+      <c r="J10" s="1">
         <v>87.52</v>
       </c>
-      <c r="K10">
-        <v>82.13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11">
+      <c r="K10" s="1">
+        <v>87.52</v>
+      </c>
+      <c r="L10" s="1">
+        <v>87.53</v>
+      </c>
+      <c r="M10" s="1">
+        <v>87.53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
       <c r="C11">
         <v>65.099999999999994</v>
       </c>
@@ -698,35 +824,35 @@
       <c r="E11">
         <v>158</v>
       </c>
-      <c r="I11">
-        <v>81.900000000000006</v>
-      </c>
-      <c r="J11">
-        <v>87.52</v>
-      </c>
-      <c r="K11">
+      <c r="J11" s="1">
+        <v>82.13</v>
+      </c>
+      <c r="K11" s="1">
+        <v>82.13</v>
+      </c>
+      <c r="L11" s="1">
         <v>87.6</v>
       </c>
-    </row>
-    <row r="12" spans="1:11">
-      <c r="I12">
-        <v>81.900000000000006</v>
-      </c>
-      <c r="J12">
-        <v>87.53</v>
-      </c>
-      <c r="K12">
+      <c r="M11" s="1">
         <v>87.6</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
-      <c r="K13">
-        <f>AVERAGE(K9,K10,K12,K11)</f>
-        <v>84.864999999999995</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="14" customHeight="1"/>
-    <row r="20" spans="1:10" ht="58" thickBot="1">
+    <row r="13" spans="1:13">
+      <c r="C13">
+        <f>AVERAGE(C9:C11)</f>
+        <v>73.95</v>
+      </c>
+      <c r="D13">
+        <f>AVERAGE(D9:D11)</f>
+        <v>84.76</v>
+      </c>
+      <c r="E13">
+        <f>AVERAGE(E9:E11)</f>
+        <v>166.79666666666665</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="14" customHeight="1"/>
+    <row r="20" spans="1:13" ht="58" thickBot="1">
       <c r="A20" s="2" t="s">
         <v>2</v>
       </c>
@@ -734,7 +860,7 @@
         <v>3</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>0</v>
@@ -742,8 +868,20 @@
       <c r="E20" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" ht="16" thickTop="1">
+      <c r="J20" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="K20" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="L20" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="M20" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="16" thickTop="1">
       <c r="C21">
         <v>110.19</v>
       </c>
@@ -753,48 +891,81 @@
       <c r="E21">
         <v>250.33</v>
       </c>
-      <c r="I21">
+      <c r="J21">
         <v>120.11</v>
       </c>
-      <c r="J21">
-        <v>100.1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10">
-      <c r="I22">
+      <c r="K21">
         <v>120.11</v>
       </c>
+      <c r="L21">
+        <v>135.13</v>
+      </c>
+      <c r="M21">
+        <v>135.13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13">
+      <c r="C22">
+        <v>135.9</v>
+      </c>
+      <c r="D22">
+        <v>100.09</v>
+      </c>
+      <c r="E22">
+        <v>241.08</v>
+      </c>
       <c r="J22">
-        <v>100.1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10">
-      <c r="I23">
-        <v>135.13</v>
+        <v>100.09</v>
+      </c>
+      <c r="K22">
+        <v>100.09</v>
+      </c>
+      <c r="L22">
+        <v>100.09</v>
+      </c>
+      <c r="M22">
+        <v>100.09</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13">
+      <c r="C23">
+        <v>124.88</v>
+      </c>
+      <c r="D23">
+        <v>100.113</v>
+      </c>
+      <c r="E23">
+        <v>230</v>
       </c>
       <c r="J23">
-        <v>90.07</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10">
-      <c r="I24">
-        <v>135.13</v>
-      </c>
-      <c r="J24">
-        <v>90.07</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="14" customHeight="1">
-      <c r="I25">
-        <f>AVERAGE(I21:I24)</f>
-        <v>127.62</v>
-      </c>
-      <c r="J25">
-        <f>AVERAGE(J21:J24)</f>
-        <v>95.084999999999994</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" ht="39" thickBot="1">
+        <v>100.113</v>
+      </c>
+      <c r="K23">
+        <v>100.113</v>
+      </c>
+      <c r="L23">
+        <v>100.113</v>
+      </c>
+      <c r="M23">
+        <v>100.113</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13">
+      <c r="C24">
+        <f>AVERAGE(C21:C23)</f>
+        <v>123.65666666666668</v>
+      </c>
+      <c r="D24">
+        <f>AVERAGE(D21:D23)</f>
+        <v>109.27433333333333</v>
+      </c>
+      <c r="E24">
+        <f>AVERAGE(E21:E23)</f>
+        <v>240.47000000000003</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="14" customHeight="1"/>
+    <row r="29" spans="1:13" ht="39" thickBot="1">
       <c r="A29" s="3" t="s">
         <v>4</v>
       </c>
@@ -802,7 +973,7 @@
         <v>3</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>0</v>
@@ -811,9 +982,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="16" thickTop="1"/>
-    <row r="34" spans="1:5" ht="14" customHeight="1"/>
-    <row r="38" spans="1:5" ht="58" thickBot="1">
+    <row r="30" spans="1:13" ht="16" thickTop="1"/>
+    <row r="34" spans="1:14" ht="14" customHeight="1"/>
+    <row r="38" spans="1:14" ht="77" thickBot="1">
       <c r="A38" s="3" t="s">
         <v>5</v>
       </c>
@@ -829,12 +1000,152 @@
       <c r="E38" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" ht="21" thickTop="1" thickBot="1">
+      <c r="G38" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H38" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J38" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="K38" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="L38" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="M38" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="N38" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" ht="21" thickTop="1" thickBot="1">
       <c r="A39" s="3"/>
-    </row>
-    <row r="40" spans="1:5" ht="16" thickTop="1">
+      <c r="B39" t="s">
+        <v>11</v>
+      </c>
+      <c r="D39">
+        <v>90.84</v>
+      </c>
+      <c r="E39">
+        <v>241.56</v>
+      </c>
+      <c r="G39">
+        <v>136</v>
+      </c>
+      <c r="H39">
+        <v>83.7</v>
+      </c>
+      <c r="J39">
+        <v>100.07</v>
+      </c>
+      <c r="K39">
+        <v>100.07</v>
+      </c>
+      <c r="L39">
+        <v>78.989999999999995</v>
+      </c>
+      <c r="M39">
+        <v>84.26</v>
+      </c>
+      <c r="N39">
+        <f>AVERAGE(J39:M39)</f>
+        <v>90.847499999999997</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" ht="16" thickTop="1">
       <c r="A40" s="1"/>
+      <c r="D40">
+        <v>90.83</v>
+      </c>
+      <c r="E40">
+        <v>299.33999999999997</v>
+      </c>
+      <c r="G40">
+        <v>122.8</v>
+      </c>
+      <c r="H40">
+        <v>209.95</v>
+      </c>
+      <c r="J40">
+        <v>100.05</v>
+      </c>
+      <c r="K40">
+        <v>100.05</v>
+      </c>
+      <c r="L40">
+        <v>84.25</v>
+      </c>
+      <c r="M40">
+        <v>78.98</v>
+      </c>
+      <c r="N40">
+        <f>AVERAGE(J40:M40)</f>
+        <v>90.83250000000001</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14">
+      <c r="D41">
+        <v>92.16</v>
+      </c>
+      <c r="E41">
+        <v>215.9</v>
+      </c>
+      <c r="G41">
+        <v>110.65</v>
+      </c>
+      <c r="H41">
+        <v>84.46</v>
+      </c>
+      <c r="J41">
+        <v>100.059</v>
+      </c>
+      <c r="K41">
+        <v>100.059</v>
+      </c>
+      <c r="L41">
+        <v>84.265000000000001</v>
+      </c>
+      <c r="M41">
+        <v>84.265000000000001</v>
+      </c>
+      <c r="N41">
+        <f>AVERAGE(J41:M41)</f>
+        <v>92.161999999999992</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14">
+      <c r="D42">
+        <v>92.215000000000003</v>
+      </c>
+      <c r="E42">
+        <v>211.16</v>
+      </c>
+      <c r="G42">
+        <v>105.76</v>
+      </c>
+      <c r="H42">
+        <v>64.2</v>
+      </c>
+      <c r="J42">
+        <v>100.12</v>
+      </c>
+      <c r="K42">
+        <v>100.12</v>
+      </c>
+      <c r="L42">
+        <v>84.31</v>
+      </c>
+      <c r="M42">
+        <v>84.31</v>
+      </c>
+      <c r="N42">
+        <f>AVERAGE(J42:M42)</f>
+        <v>92.215000000000003</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
adding excel figure and updates in excel
git-svn-id: file://localhost/tmp/svn2git/svn@5371 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/troy/pstar/new_results.xlsx
+++ b/papers/troy/pstar/new_results.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="30">
   <si>
     <t>wu-runtime avg</t>
   </si>
@@ -85,6 +85,30 @@
   </si>
   <si>
     <t>redis://cyder.cct.lsu.edu:2525</t>
+  </si>
+  <si>
+    <t>1 nodes(4 Bfast tasks per node)</t>
+  </si>
+  <si>
+    <t>TROY-CONDOR</t>
+  </si>
+  <si>
+    <t>TROY-BJ+DIANE</t>
+  </si>
+  <si>
+    <t>TROY+STARTUP</t>
+  </si>
+  <si>
+    <t>BFAST-Runtime</t>
+  </si>
+  <si>
+    <t>Total Time</t>
+  </si>
+  <si>
+    <t>Overhead</t>
+  </si>
+  <si>
+    <t>TROY+AGENT STARTUP</t>
   </si>
 </sst>
 </file>
@@ -169,7 +193,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="123">
+  <cellStyleXfs count="175">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -293,8 +317,60 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyAlignment="1">
@@ -311,8 +387,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
   </cellXfs>
-  <cellStyles count="123">
+  <cellStyles count="175">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -374,6 +451,32 @@
     <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -435,11 +538,403 @@
     <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.118863549068562"/>
+          <c:y val="0.0357634112792297"/>
+          <c:w val="0.832387491197747"/>
+          <c:h val="0.894507251242838"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$68</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>TROY+AGENT STARTUP</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="50000"/>
+                <a:lumOff val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$69:$A$72</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>TROY-BJ</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>TROY-DIANE</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>TROY-CONDOR</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>TROY-BJ+DIANE</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$69:$B$72</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>73.95</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>123.65</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>37.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>91.74</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$68</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>BFAST-Runtime</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$69:$A$72</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>TROY-BJ</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>TROY-DIANE</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>TROY-CONDOR</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>TROY-BJ+DIANE</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$69:$C$72</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>84.76</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>109.27</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>51.65</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>97.46</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$68</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Overhead</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="bg1">
+                <a:lumMod val="95000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$69:$A$72</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>TROY-BJ</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>TROY-DIANE</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>TROY-CONDOR</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>TROY-BJ+DIANE</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$69:$D$72</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>8.08</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.55</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.77</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>33.67</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="651853016"/>
+        <c:axId val="652701128"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="651853016"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="652701128"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="652701128"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time to</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Completion(sec)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.0101626016260163"/>
+              <c:y val="0.335940170477315"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="651853016"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="25400">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.591494942705333"/>
+          <c:y val="0.0980071266882561"/>
+          <c:w val="0.230623679661993"/>
+          <c:h val="0.165746190254416"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1612900</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>69850</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
+      <xdr:row>99</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -764,16 +1259,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N44"/>
+  <dimension ref="A1:N72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="B75" sqref="B75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="17.5" customWidth="1"/>
-    <col min="2" max="2" width="32.6640625" customWidth="1"/>
+    <col min="2" max="2" width="35.5" customWidth="1"/>
     <col min="3" max="3" width="40.1640625" customWidth="1"/>
     <col min="4" max="4" width="24.1640625" customWidth="1"/>
   </cols>
@@ -1023,7 +1518,7 @@
         <v>4</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>9</v>
@@ -1295,9 +1790,184 @@
         <v>97.461666666666673</v>
       </c>
     </row>
+    <row r="57" spans="1:8" ht="20" thickBot="1">
+      <c r="A57" s="8"/>
+      <c r="B57" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C57" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D57" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E57" s="8"/>
+      <c r="F57" s="8"/>
+      <c r="G57" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H57" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" ht="16" thickTop="1">
+      <c r="A58" t="s">
+        <v>1</v>
+      </c>
+      <c r="B58">
+        <v>73.95</v>
+      </c>
+      <c r="C58">
+        <v>84.76</v>
+      </c>
+      <c r="D58">
+        <v>166.79</v>
+      </c>
+      <c r="G58">
+        <f>-B58-C58+D58</f>
+        <v>8.0799999999999841</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8">
+      <c r="A59" t="s">
+        <v>2</v>
+      </c>
+      <c r="B59">
+        <v>123.65</v>
+      </c>
+      <c r="C59">
+        <v>109.27</v>
+      </c>
+      <c r="D59">
+        <v>240.47</v>
+      </c>
+      <c r="G59">
+        <f>D59-SUM(B59+C59)</f>
+        <v>7.5499999999999829</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8">
+      <c r="A60" t="s">
+        <v>23</v>
+      </c>
+      <c r="B60">
+        <v>37.299999999999997</v>
+      </c>
+      <c r="C60">
+        <v>51.65</v>
+      </c>
+      <c r="D60">
+        <v>97.72</v>
+      </c>
+      <c r="G60">
+        <f>D60-(B60+C60)</f>
+        <v>8.7700000000000102</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8">
+      <c r="A61" t="s">
+        <v>24</v>
+      </c>
+      <c r="B61">
+        <v>91.74</v>
+      </c>
+      <c r="C61">
+        <v>97.46</v>
+      </c>
+      <c r="D61">
+        <v>222.87</v>
+      </c>
+      <c r="G61">
+        <f>D61-(C61+B61)</f>
+        <v>33.670000000000016</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
+      <c r="B68" t="s">
+        <v>29</v>
+      </c>
+      <c r="C68" t="s">
+        <v>26</v>
+      </c>
+      <c r="D68" t="s">
+        <v>28</v>
+      </c>
+      <c r="E68" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
+      <c r="A69" t="s">
+        <v>1</v>
+      </c>
+      <c r="B69">
+        <v>73.95</v>
+      </c>
+      <c r="C69">
+        <v>84.76</v>
+      </c>
+      <c r="D69">
+        <v>8.08</v>
+      </c>
+      <c r="E69">
+        <v>166.79</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
+      <c r="A70" t="s">
+        <v>2</v>
+      </c>
+      <c r="B70">
+        <v>123.65</v>
+      </c>
+      <c r="C70">
+        <v>109.27</v>
+      </c>
+      <c r="D70">
+        <v>7.55</v>
+      </c>
+      <c r="E70">
+        <v>240.47</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5">
+      <c r="A71" t="s">
+        <v>23</v>
+      </c>
+      <c r="B71">
+        <v>37.299999999999997</v>
+      </c>
+      <c r="C71">
+        <v>51.65</v>
+      </c>
+      <c r="D71">
+        <v>8.77</v>
+      </c>
+      <c r="E71">
+        <v>97.72</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5">
+      <c r="A72" t="s">
+        <v>24</v>
+      </c>
+      <c r="B72">
+        <v>91.74</v>
+      </c>
+      <c r="C72">
+        <v>97.46</v>
+      </c>
+      <c r="D72">
+        <v>33.67</v>
+      </c>
+      <c r="E72">
+        <v>222.87</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
updated figure along lines of discussion's with Andre
git-svn-id: file://localhost/tmp/svn2git/svn@5374 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/troy/pstar/new_results.xlsx
+++ b/papers/troy/pstar/new_results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1260" yWindow="0" windowWidth="25600" windowHeight="16360" tabRatio="189"/>
+    <workbookView xWindow="980" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="189"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -87,9 +87,6 @@
     <t>redis://cyder.cct.lsu.edu:2525</t>
   </si>
   <si>
-    <t>1 nodes(4 Bfast tasks per node)</t>
-  </si>
-  <si>
     <t>TROY-CONDOR</t>
   </si>
   <si>
@@ -109,6 +106,9 @@
   </si>
   <si>
     <t>TROY+AGENT STARTUP</t>
+  </si>
+  <si>
+    <t>1 node(4 Bfast tasks per node)</t>
   </si>
 </sst>
 </file>
@@ -193,10 +193,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="175">
+  <cellStyleXfs count="183">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -389,7 +397,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
   </cellXfs>
-  <cellStyles count="175">
+  <cellStyles count="183">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -477,6 +485,10 @@
     <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -564,6 +576,10 @@
     <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -723,7 +739,7 @@
                   <c:v>51.65</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>97.46</c:v>
+                  <c:v>77.45</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -787,7 +803,7 @@
                   <c:v>8.77</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>33.67</c:v>
+                  <c:v>53.68</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -803,11 +819,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="651853016"/>
-        <c:axId val="652701128"/>
+        <c:axId val="565872344"/>
+        <c:axId val="535558376"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="651853016"/>
+        <c:axId val="565872344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -816,7 +832,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="652701128"/>
+        <c:crossAx val="535558376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -824,7 +840,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="652701128"/>
+        <c:axId val="535558376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -865,7 +881,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="651853016"/>
+        <c:crossAx val="565872344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -882,8 +898,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.591494942705333"/>
-          <c:y val="0.0980071266882561"/>
+          <c:x val="0.538649414250048"/>
+          <c:y val="0.0649947470458902"/>
           <c:w val="0.230623679661993"/>
           <c:h val="0.165746190254416"/>
         </c:manualLayout>
@@ -1262,7 +1278,7 @@
   <dimension ref="A1:N72"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="B75" sqref="B75"/>
+      <selection activeCell="C72" sqref="C72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1518,7 +1534,7 @@
         <v>4</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>9</v>
@@ -1793,21 +1809,21 @@
     <row r="57" spans="1:8" ht="20" thickBot="1">
       <c r="A57" s="8"/>
       <c r="B57" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C57" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C57" s="8" t="s">
+      <c r="D57" s="8" t="s">
         <v>26</v>
-      </c>
-      <c r="D57" s="8" t="s">
-        <v>27</v>
       </c>
       <c r="E57" s="8"/>
       <c r="F57" s="8"/>
       <c r="G57" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H57" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="58" spans="1:8" ht="16" thickTop="1">
@@ -1848,7 +1864,7 @@
     </row>
     <row r="60" spans="1:8">
       <c r="A60" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B60">
         <v>37.299999999999997</v>
@@ -1866,34 +1882,34 @@
     </row>
     <row r="61" spans="1:8">
       <c r="A61" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B61">
         <v>91.74</v>
       </c>
       <c r="C61">
-        <v>97.46</v>
+        <v>77.45</v>
       </c>
       <c r="D61">
         <v>222.87</v>
       </c>
       <c r="G61">
         <f>D61-(C61+B61)</f>
-        <v>33.670000000000016</v>
+        <v>53.680000000000007</v>
       </c>
     </row>
     <row r="68" spans="1:5">
       <c r="B68" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C68" t="s">
+        <v>25</v>
+      </c>
+      <c r="D68" t="s">
+        <v>27</v>
+      </c>
+      <c r="E68" t="s">
         <v>26</v>
-      </c>
-      <c r="D68" t="s">
-        <v>28</v>
-      </c>
-      <c r="E68" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="69" spans="1:5">
@@ -1932,7 +1948,7 @@
     </row>
     <row r="71" spans="1:5">
       <c r="A71" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B71">
         <v>37.299999999999997</v>
@@ -1949,16 +1965,16 @@
     </row>
     <row r="72" spans="1:5">
       <c r="A72" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B72">
         <v>91.74</v>
       </c>
       <c r="C72">
-        <v>97.46</v>
+        <v>77.45</v>
       </c>
       <c r="D72">
-        <v>33.67</v>
+        <v>53.68</v>
       </c>
       <c r="E72">
         <v>222.87</v>

</xml_diff>

<commit_message>
updated sheet with figure
git-svn-id: file://localhost/tmp/svn2git/svn@5380 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/troy/pstar/new_results.xlsx
+++ b/papers/troy/pstar/new_results.xlsx
@@ -608,10 +608,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.118863549068562"/>
-          <c:y val="0.0357634112792297"/>
+          <c:x val="0.124830116700806"/>
+          <c:y val="0.0362544583112882"/>
           <c:w val="0.832387491197747"/>
-          <c:h val="0.894507251242838"/>
+          <c:h val="0.864467710310915"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -819,11 +819,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="565872344"/>
-        <c:axId val="535558376"/>
+        <c:axId val="591350632"/>
+        <c:axId val="591353608"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="565872344"/>
+        <c:axId val="591350632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -832,7 +832,19 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="535558376"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2300">
+                <a:latin typeface="Droid Sans Mono"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="591353608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -840,7 +852,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="535558376"/>
+        <c:axId val="591353608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -853,17 +865,16 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="2600" b="0" i="0">
+                    <a:latin typeface="Droid Sans Mono"/>
+                  </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Time to</a:t>
+                  <a:rPr lang="en-US" sz="2600" b="0" i="0">
+                    <a:latin typeface="Droid Sans Mono"/>
+                  </a:rPr>
+                  <a:t>Time to Completion(sec)</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> Completion(sec)</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -871,8 +882,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.0101626016260163"/>
-              <c:y val="0.335940170477315"/>
+              <c:x val="0.00538937853532031"/>
+              <c:y val="0.168601537456039"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -881,7 +892,19 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="565872344"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2000">
+                <a:latin typeface="Droid Sans Mono"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="591350632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -898,18 +921,40 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.538649414250048"/>
-          <c:y val="0.0649947470458902"/>
-          <c:w val="0.230623679661993"/>
-          <c:h val="0.165746190254416"/>
+          <c:x val="0.502849867513578"/>
+          <c:y val="0.000651582583797579"/>
+          <c:w val="0.416781237667487"/>
+          <c:h val="0.262260876907813"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="2600" b="0" i="0">
+              <a:latin typeface="Droid Sans Mono"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1600"/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
@@ -928,10 +973,10 @@
       <xdr:rowOff>69850</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>254000</xdr:colOff>
-      <xdr:row>99</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>520700</xdr:colOff>
+      <xdr:row>117</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1277,8 +1322,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="C72" sqref="C72"/>
+    <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
+      <selection activeCell="D121" sqref="D121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
adding table with with std dev data
git-svn-id: file://localhost/tmp/svn2git/svn@5385 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/troy/pstar/new_results.xlsx
+++ b/papers/troy/pstar/new_results.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="34">
   <si>
     <t>wu-runtime avg</t>
   </si>
@@ -93,9 +93,6 @@
     <t>TROY-BJ+DIANE</t>
   </si>
   <si>
-    <t>TROY+STARTUP</t>
-  </si>
-  <si>
     <t>BFAST-Runtime</t>
   </si>
   <si>
@@ -109,13 +106,28 @@
   </si>
   <si>
     <t>1 node(4 Bfast tasks per node)</t>
+  </si>
+  <si>
+    <t>stddev-TROY+AGENT STARTUP</t>
+  </si>
+  <si>
+    <t>stddev-BFAST-Runtime</t>
+  </si>
+  <si>
+    <t>stddev-Overhead</t>
+  </si>
+  <si>
+    <t>stddev-Totoal time</t>
+  </si>
+  <si>
+    <t>Table with std dev</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -161,6 +173,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color rgb="FF1F497D"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -175,7 +195,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -192,8 +212,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color rgb="FF4F81BD"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="183">
+  <cellStyleXfs count="235">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -377,8 +406,60 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyAlignment="1">
@@ -395,9 +476,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="183">
+  <cellStyles count="235">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -489,6 +573,32 @@
     <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="200" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="202" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="204" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="206" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="208" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="210" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="212" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="214" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="216" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="218" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="220" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="222" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="224" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="226" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="228" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="230" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="232" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="234" builtinId="9" hidden="1"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -580,6 +690,32 @@
     <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="189" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="191" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="193" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="195" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="197" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="199" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="201" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="203" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="205" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="207" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="209" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="211" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="213" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="215" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="217" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="219" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="221" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="223" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="225" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="227" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="229" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="231" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="233" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -819,16 +955,17 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="591350632"/>
-        <c:axId val="591353608"/>
+        <c:axId val="790082184"/>
+        <c:axId val="790249704"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="591350632"/>
+        <c:axId val="790082184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -844,7 +981,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="591353608"/>
+        <c:crossAx val="790249704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -852,7 +989,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="591353608"/>
+        <c:axId val="790249704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -904,7 +1041,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="591350632"/>
+        <c:crossAx val="790082184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -968,15 +1105,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1612900</xdr:colOff>
-      <xdr:row>75</xdr:row>
-      <xdr:rowOff>69850</xdr:rowOff>
+      <xdr:colOff>1752600</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>520700</xdr:colOff>
-      <xdr:row>117</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:colOff>660400</xdr:colOff>
+      <xdr:row>125</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1320,10 +1457,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N72"/>
+  <dimension ref="A1:N74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
-      <selection activeCell="D121" sqref="D121"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="C66" sqref="C66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1455,6 +1592,20 @@
         <v>166.79666666666665</v>
       </c>
     </row>
+    <row r="14" spans="1:13">
+      <c r="C14">
+        <f>STDEV(C9:C11)</f>
+        <v>8.1144377500847273</v>
+      </c>
+      <c r="D14">
+        <f>STDEV(D9:D11)</f>
+        <v>2.8113342028296766</v>
+      </c>
+      <c r="E14">
+        <f>STDEV(E9:E11)</f>
+        <v>8.0512131591042486</v>
+      </c>
+    </row>
     <row r="15" spans="1:13" ht="14" customHeight="1"/>
     <row r="20" spans="1:13" ht="39" thickBot="1">
       <c r="A20" s="2" t="s">
@@ -1568,7 +1719,20 @@
         <v>240.47000000000003</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="14" customHeight="1"/>
+    <row r="25" spans="1:13" ht="14" customHeight="1">
+      <c r="C25">
+        <f>STDEV(C21:C23)</f>
+        <v>12.898582609470447</v>
+      </c>
+      <c r="D25">
+        <f>STDEV(D21:D23)</f>
+        <v>15.88781754468919</v>
+      </c>
+      <c r="E25">
+        <f>STDEV(E21:E23)</f>
+        <v>10.178717993932249</v>
+      </c>
+    </row>
     <row r="28" spans="1:13">
       <c r="C28" t="s">
         <v>21</v>
@@ -1579,7 +1743,7 @@
         <v>4</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>9</v>
@@ -1662,6 +1826,20 @@
         <v>97.726666666666674</v>
       </c>
     </row>
+    <row r="35" spans="1:14">
+      <c r="C35">
+        <f>STDEV(C30:C32)</f>
+        <v>0.49166384179979533</v>
+      </c>
+      <c r="D35">
+        <f>STDEV(D30:D32)</f>
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <f>STDEV(E30:E32)</f>
+        <v>3.0023712850567499</v>
+      </c>
+    </row>
     <row r="37" spans="1:14">
       <c r="C37" t="s">
         <v>19</v>
@@ -1851,27 +2029,54 @@
         <v>97.461666666666673</v>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="20" thickBot="1">
-      <c r="A57" s="8"/>
-      <c r="B57" s="8" t="s">
+    <row r="45" spans="1:14">
+      <c r="D45">
+        <f>STDEV(D39,D41,D42)</f>
+        <v>0.77846537067061017</v>
+      </c>
+      <c r="E45">
+        <f>STDEV(E39,E41:E42)</f>
+        <v>16.355749244022221</v>
+      </c>
+      <c r="H45">
+        <f>STDEV(H39,H41,H42)</f>
+        <v>11.484012074764271</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" ht="20" thickBot="1">
+      <c r="A55" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" ht="16" thickTop="1"/>
+    <row r="57" spans="1:9" ht="58" thickBot="1">
+      <c r="A57" s="5"/>
+      <c r="B57" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D57" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C57" s="8" t="s">
+      <c r="E57" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F57" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G57" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H57" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D57" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="E57" s="8"/>
-      <c r="F57" s="8"/>
-      <c r="G57" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="H57" s="8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" ht="16" thickTop="1">
+      <c r="I57" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" ht="16" thickTop="1">
       <c r="A58" t="s">
         <v>1</v>
       </c>
@@ -1879,17 +2084,28 @@
         <v>73.95</v>
       </c>
       <c r="C58">
+        <v>8.11</v>
+      </c>
+      <c r="D58">
         <v>84.76</v>
       </c>
-      <c r="D58">
+      <c r="E58">
+        <v>2.81</v>
+      </c>
+      <c r="F58">
+        <v>8.08</v>
+      </c>
+      <c r="G58">
+        <v>2.87</v>
+      </c>
+      <c r="H58">
         <v>166.79</v>
       </c>
-      <c r="G58">
-        <f>-B58-C58+D58</f>
-        <v>8.0799999999999841</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8">
+      <c r="I58">
+        <v>8.0500000000000007</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9">
       <c r="A59" t="s">
         <v>2</v>
       </c>
@@ -1897,17 +2113,28 @@
         <v>123.65</v>
       </c>
       <c r="C59">
+        <v>12.89</v>
+      </c>
+      <c r="D59">
         <v>109.27</v>
       </c>
-      <c r="D59">
+      <c r="E59">
+        <v>15.88</v>
+      </c>
+      <c r="F59">
+        <v>7.55</v>
+      </c>
+      <c r="G59">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="H59">
         <v>240.47</v>
       </c>
-      <c r="G59">
-        <f>D59-SUM(B59+C59)</f>
-        <v>7.5499999999999829</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8">
+      <c r="I59">
+        <v>10.17</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9">
       <c r="A60" t="s">
         <v>22</v>
       </c>
@@ -1915,17 +2142,28 @@
         <v>37.299999999999997</v>
       </c>
       <c r="C60">
+        <v>0.49</v>
+      </c>
+      <c r="D60">
         <v>51.65</v>
       </c>
-      <c r="D60">
+      <c r="E60">
+        <v>0</v>
+      </c>
+      <c r="F60">
+        <v>8.77</v>
+      </c>
+      <c r="G60">
+        <v>2.5099999999999998</v>
+      </c>
+      <c r="H60">
         <v>97.72</v>
       </c>
-      <c r="G60">
-        <f>D60-(B60+C60)</f>
-        <v>8.7700000000000102</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8">
+      <c r="I60">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9">
       <c r="A61" t="s">
         <v>23</v>
       </c>
@@ -1933,31 +2171,42 @@
         <v>91.74</v>
       </c>
       <c r="C61">
+        <v>0.77</v>
+      </c>
+      <c r="D61">
         <v>77.45</v>
       </c>
-      <c r="D61">
+      <c r="E61">
+        <v>16.350000000000001</v>
+      </c>
+      <c r="F61">
+        <v>53.68</v>
+      </c>
+      <c r="G61">
+        <v>5.64</v>
+      </c>
+      <c r="H61">
         <v>222.87</v>
       </c>
-      <c r="G61">
-        <f>D61-(C61+B61)</f>
-        <v>53.680000000000007</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5">
+      <c r="I61">
+        <v>11.48</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11">
       <c r="B68" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C68" t="s">
+        <v>24</v>
+      </c>
+      <c r="D68" t="s">
+        <v>26</v>
+      </c>
+      <c r="E68" t="s">
         <v>25</v>
       </c>
-      <c r="D68" t="s">
-        <v>27</v>
-      </c>
-      <c r="E68" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5">
+    </row>
+    <row r="69" spans="1:11">
       <c r="A69" t="s">
         <v>1</v>
       </c>
@@ -1973,8 +2222,21 @@
       <c r="E69">
         <v>166.79</v>
       </c>
-    </row>
-    <row r="70" spans="1:5">
+      <c r="G69">
+        <v>8.11</v>
+      </c>
+      <c r="H69">
+        <v>2.81</v>
+      </c>
+      <c r="I69">
+        <v>8.0500000000000007</v>
+      </c>
+      <c r="K69">
+        <f>I69-H69-G69</f>
+        <v>-2.8699999999999992</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11">
       <c r="A70" t="s">
         <v>2</v>
       </c>
@@ -1990,8 +2252,21 @@
       <c r="E70">
         <v>240.47</v>
       </c>
-    </row>
-    <row r="71" spans="1:5">
+      <c r="G70">
+        <v>12.89</v>
+      </c>
+      <c r="H70">
+        <v>15.88</v>
+      </c>
+      <c r="I70">
+        <v>10.17</v>
+      </c>
+      <c r="K70">
+        <f>I70-H70-G70</f>
+        <v>-18.600000000000001</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11">
       <c r="A71" t="s">
         <v>22</v>
       </c>
@@ -2007,8 +2282,21 @@
       <c r="E71">
         <v>97.72</v>
       </c>
-    </row>
-    <row r="72" spans="1:5">
+      <c r="G71">
+        <v>0.49</v>
+      </c>
+      <c r="H71">
+        <v>0</v>
+      </c>
+      <c r="I71">
+        <v>3</v>
+      </c>
+      <c r="K71">
+        <f>I71-G71-H71</f>
+        <v>2.5099999999999998</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11">
       <c r="A72" t="s">
         <v>23</v>
       </c>
@@ -2024,7 +2312,21 @@
       <c r="E72">
         <v>222.87</v>
       </c>
-    </row>
+      <c r="G72">
+        <v>0.77</v>
+      </c>
+      <c r="H72">
+        <v>16.350000000000001</v>
+      </c>
+      <c r="I72">
+        <v>11.48</v>
+      </c>
+      <c r="K72">
+        <f>I72-H72-G72</f>
+        <v>-5.6400000000000006</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" s="8" customFormat="1"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>